<commit_message>
General review. Bug fix on coordinates
</commit_message>
<xml_diff>
--- a/layerCoordinates_left.xlsx
+++ b/layerCoordinates_left.xlsx
@@ -427,7 +427,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -437,7 +437,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -447,7 +447,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -457,7 +457,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -467,7 +467,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -487,7 +487,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -537,7 +537,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -557,7 +557,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -567,7 +567,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -597,7 +597,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -607,7 +607,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -617,7 +617,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -637,7 +637,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -647,7 +647,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -687,7 +687,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -697,7 +697,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -707,7 +707,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -787,7 +787,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -797,7 +797,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -817,7 +817,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -827,7 +827,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -847,7 +847,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -857,7 +857,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -867,7 +867,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -887,7 +887,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -907,7 +907,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -917,7 +917,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -927,7 +927,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -937,7 +937,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -957,7 +957,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -967,7 +967,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -977,7 +977,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -987,7 +987,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -997,7 +997,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1017,7 +1017,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1027,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1077,7 +1077,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1137,7 +1137,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1187,7 +1187,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1217,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1237,7 +1237,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1247,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1417,7 +1417,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1427,7 +1427,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1477,7 +1477,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1497,7 +1497,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1567,7 +1567,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1587,7 +1587,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1627,7 +1627,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1667,7 +1667,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1717,7 +1717,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1767,7 +1767,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1797,7 +1797,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1957,7 +1957,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1977,7 +1977,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1987,7 +1987,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -1997,7 +1997,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2027,7 +2027,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>[(-0.3, 160.0), (-0.3, 159.88), (-4.255, 160.0), (-4.255, 159.88), (-4.255, 160.0), (-4.255, 159.86), (-15.746, 160.0), (-15.746, 159.86), (-0.3, 159.88), (-0.3, 159.58), (-4.255, 159.88), (-4.255, 159.74), (-4.255, 159.74), (-15.746, 159.74), (-4.255, 159.86), (-15.746, 159.74)]</t>
+          <t>[(-0.3, 160.0), (-0.3, 159.88), (-4.255, 160.0), (-4.255, 159.88), (-4.255, 160.0), (-4.255, 159.86), (-15.746, 160.0), (-15.746, 159.86), (-0.3, 159.88), (-0.3, 159.58), (-4.255, 159.88), (-4.255, 159.74), (-4.255, 159.86), (-4.255, 159.74), (-15.746, 159.86), (-15.746, 159.74)]</t>
         </is>
       </c>
     </row>
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2047,7 +2047,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2067,7 +2067,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2137,7 +2137,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2257,7 +2257,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2367,7 +2367,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2487,7 +2487,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2547,7 +2547,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2567,7 +2567,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2577,7 +2577,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>[(-0.3, 218.0), (-0.3, 217.89), (-6.083, 218.0), (-6.083, 217.89), (-6.083, 218.0), (-6.083, 217.75), (-9.456, 218.0), (-9.456, 217.75), (-0.3, 217.89), (-0.3, 217.73), (-6.083, 217.89), (-6.083, 217.64), (-6.083, 217.64), (-9.456, 217.51), (-6.083, 217.75), (-9.456, 217.51)]</t>
+          <t>[(-0.3, 218.0), (-0.3, 217.89), (-6.083, 218.0), (-6.083, 217.89), (-6.083, 218.0), (-6.083, 217.75), (-9.456, 218.0), (-9.456, 217.75), (-0.3, 217.89), (-0.3, 217.73), (-6.083, 217.89), (-6.083, 217.64), (-6.083, 217.75), (-6.083, 217.64), (-9.456, 217.75), (-9.456, 217.51)]</t>
         </is>
       </c>
     </row>
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>[(-0.3, 219.0), (-0.3, 218.89), (-7.801, 219.0), (-7.801, 218.89), (-7.801, 219.0), (-7.801, 218.72), (-11.196, 219.0), (-11.196, 218.72), (-0.3, 218.89), (-0.3, 218.72), (-7.801, 218.89), (-7.801, 218.59), (-7.801, 218.59), (-11.196, 218.44), (-7.801, 218.72), (-11.196, 218.44)]</t>
+          <t>[(-0.3, 219.0), (-0.3, 218.89), (-7.801, 219.0), (-7.801, 218.89), (-7.801, 219.0), (-7.801, 218.72), (-11.196, 219.0), (-11.196, 218.72), (-0.3, 218.89), (-0.3, 218.72), (-7.801, 218.89), (-7.801, 218.59), (-7.801, 218.72), (-7.801, 218.59), (-11.196, 218.72), (-11.196, 218.44)]</t>
         </is>
       </c>
     </row>
@@ -2627,7 +2627,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>[(-0.3, 220.0), (-0.3, 219.86), (-9.188, 220.0), (-9.188, 219.86), (-9.188, 220.0), (-9.188, 219.71), (-12.555, 220.0), (-12.555, 219.71), (-0.3, 219.86), (-0.3, 219.69), (-9.188, 219.86), (-9.188, 219.56), (-9.188, 219.56), (-12.555, 219.42), (-9.188, 219.71), (-12.555, 219.42)]</t>
+          <t>[(-0.3, 220.0), (-0.3, 219.86), (-9.188, 220.0), (-9.188, 219.86), (-9.188, 220.0), (-9.188, 219.71), (-12.555, 220.0), (-12.555, 219.71), (-0.3, 219.86), (-0.3, 219.69), (-9.188, 219.86), (-9.188, 219.56), (-9.188, 219.71), (-9.188, 219.56), (-12.555, 219.71), (-12.555, 219.42)]</t>
         </is>
       </c>
     </row>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>[(-0.3, 221.0), (-0.3, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-13.47, 221.0), (-13.47, 220.76), (-0.3, 220.76), (-0.3, 220.53), (-10.073, 220.76), (-10.073, 220.64), (-10.073, 220.64), (-13.47, 220.53), (-10.073, 220.76), (-13.47, 220.53)]</t>
+          <t>[(-0.3, 221.0), (-0.3, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-10.073, 221.0), (-10.073, 220.76), (-13.47, 221.0), (-13.47, 220.76), (-0.3, 220.76), (-0.3, 220.53), (-10.073, 220.76), (-10.073, 220.64), (-10.073, 220.76), (-10.073, 220.64), (-13.47, 220.76), (-13.47, 220.53)]</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2667,7 +2667,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2677,7 +2677,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2707,7 +2707,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2757,7 +2757,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2767,7 +2767,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2777,7 +2777,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2787,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2837,7 +2837,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>[(-0.3, 243.0), (-0.3, 242.85), (-3.224, 243.0), (-3.224, 242.85), (-3.224, 243.0), (-3.224, 242.83), (-9.022, 243.0), (-9.022, 242.83), (-0.3, 242.85), (-0.3, 242.71), (-3.224, 242.85), (-3.224, 242.7), (-3.224, 242.7), (-9.022, 242.66), (-3.224, 242.83), (-9.022, 242.66)]</t>
+          <t>[(-0.3, 243.0), (-0.3, 242.85), (-3.224, 243.0), (-3.224, 242.85), (-3.224, 243.0), (-3.224, 242.83), (-9.022, 243.0), (-9.022, 242.83), (-0.3, 242.85), (-0.3, 242.71), (-3.224, 242.85), (-3.224, 242.7), (-3.224, 242.83), (-3.224, 242.7), (-9.022, 242.83), (-9.022, 242.66)]</t>
         </is>
       </c>
     </row>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>[(-0.3, 244.0), (-0.3, 243.83), (-3.053, 244.0), (-3.053, 243.83), (-3.053, 244.0), (-3.053, 243.77), (-9.943, 244.0), (-9.943, 243.77), (-0.3, 243.83), (-0.3, 243.67), (-3.053, 243.83), (-3.053, 243.66), (-3.053, 243.66), (-9.943, 243.47), (-3.053, 243.77), (-9.943, 243.47)]</t>
+          <t>[(-0.3, 244.0), (-0.3, 243.83), (-3.053, 244.0), (-3.053, 243.83), (-3.053, 244.0), (-3.053, 243.77), (-9.943, 244.0), (-9.943, 243.77), (-0.3, 243.83), (-0.3, 243.67), (-3.053, 243.83), (-3.053, 243.66), (-3.053, 243.77), (-3.053, 243.66), (-9.943, 243.77), (-9.943, 243.47)]</t>
         </is>
       </c>
     </row>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>[(-0.3, 245.0), (-0.3, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-9.696, 245.0), (-9.696, 244.73), (-0.3, 244.83), (-0.3, 244.69), (-2.817, 244.83), (-2.817, 244.66), (-2.817, 244.66), (-9.696, 244.46), (-2.817, 244.83), (-9.696, 244.46)]</t>
+          <t>[(-0.3, 245.0), (-0.3, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-2.817, 245.0), (-2.817, 244.83), (-9.696, 245.0), (-9.696, 244.73), (-0.3, 244.83), (-0.3, 244.69), (-2.817, 244.83), (-2.817, 244.66), (-2.817, 244.83), (-2.817, 244.66), (-9.696, 244.73), (-9.696, 244.46)]</t>
         </is>
       </c>
     </row>
@@ -2887,7 +2887,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>[(-0.3, 246.0), (-0.3, 245.84), (-2.868, 246.0), (-2.868, 245.84), (-2.868, 246.0), (-2.868, 245.81), (-9.652, 246.0), (-9.652, 245.81), (-0.3, 245.84), (-0.3, 245.73), (-2.868, 245.84), (-2.868, 245.68), (-2.868, 245.68), (-9.652, 245.51), (-2.868, 245.81), (-9.652, 245.51)]</t>
+          <t>[(-0.3, 246.0), (-0.3, 245.84), (-2.868, 246.0), (-2.868, 245.84), (-2.868, 246.0), (-2.868, 245.81), (-9.652, 246.0), (-9.652, 245.81), (-0.3, 245.84), (-0.3, 245.73), (-2.868, 245.84), (-2.868, 245.68), (-2.868, 245.81), (-2.868, 245.68), (-9.652, 245.81), (-9.652, 245.51)]</t>
         </is>
       </c>
     </row>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2917,7 +2917,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -2927,7 +2927,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>[(-0.3, 250.0), (-0.3, 249.89), (-3.599, 250.0), (-3.599, 249.89), (-3.599, 250.0), (-3.599, 249.79), (-7.357, 250.0), (-7.357, 249.79), (-0.3, 249.89), (-0.3, 249.74), (-3.599, 249.89), (-3.599, 249.67), (-3.599, 249.67), (-7.357, 249.59), (-3.599, 249.79), (-7.357, 249.59)]</t>
+          <t>[(-0.3, 250.0), (-0.3, 249.89), (-3.599, 250.0), (-3.599, 249.89), (-3.599, 250.0), (-3.599, 249.79), (-7.357, 250.0), (-7.357, 249.79), (-0.3, 249.89), (-0.3, 249.74), (-3.599, 249.89), (-3.599, 249.67), (-3.599, 249.79), (-3.599, 249.67), (-7.357, 249.79), (-7.357, 249.59)]</t>
         </is>
       </c>
     </row>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>[(-0.3, 251.0), (-0.3, 250.79), (-3.931, 251.0), (-3.931, 250.79), (-3.931, 251.0), (-3.931, 250.71), (-11.377, 251.0), (-11.377, 250.71), (-0.3, 250.79), (-0.3, 250.63), (-3.931, 250.79), (-3.931, 250.58), (-3.931, 250.58), (-11.377, 250.42), (-3.931, 250.71), (-11.377, 250.42)]</t>
+          <t>[(-0.3, 251.0), (-0.3, 250.79), (-3.931, 251.0), (-3.931, 250.79), (-3.931, 251.0), (-3.931, 250.71), (-11.377, 251.0), (-11.377, 250.71), (-0.3, 250.79), (-0.3, 250.63), (-3.931, 250.79), (-3.931, 250.58), (-3.931, 250.71), (-3.931, 250.58), (-11.377, 250.71), (-11.377, 250.42)]</t>
         </is>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>[(-0.3, 252.0), (-0.3, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-7.959, 252.0), (-7.959, 251.85), (-0.3, 251.85), (-0.3, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-4.19, 251.7), (-7.959, 251.7), (-4.19, 251.85), (-7.959, 251.7), (-0.3, 251.7), (-0.3, 251.55), (-4.19, 251.7), (-4.19, 251.56), (-4.19, 251.7), (-7.959, 251.7), (-4.19, 251.85), (-7.959, 251.7)]</t>
+          <t>[(-0.3, 252.0), (-0.3, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-4.19, 252.0), (-4.19, 251.85), (-7.959, 252.0), (-7.959, 251.85), (-0.3, 251.85), (-0.3, 251.7), (-4.19, 251.85), (-4.19, 251.7), (-4.19, 251.7), (-4.19, 251.7), (-7.959, 251.85), (-7.959, 251.7), (-0.3, 251.7), (-0.3, 251.55), (-4.19, 251.7), (-4.19, 251.56), (-4.19, 251.7), (-4.19, 251.7), (-7.959, 251.85), (-7.959, 251.7)]</t>
         </is>
       </c>
     </row>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>[(-0.3, 253.0), (-0.3, 252.83), (-5.084, 253.0), (-5.084, 252.83), (-5.084, 253.0), (-5.084, 252.85), (-8.801, 253.0), (-8.801, 252.85), (-0.3, 252.83), (-0.3, 252.66), (-5.084, 252.83), (-5.084, 252.66), (-5.084, 252.7), (-8.801, 252.7), (-5.084, 252.85), (-8.801, 252.7), (-0.3, 252.66), (-0.3, 252.51), (-5.084, 252.66), (-5.084, 252.55), (-5.084, 252.7), (-8.801, 252.7), (-5.084, 252.85), (-8.801, 252.7)]</t>
+          <t>[(-0.3, 253.0), (-0.3, 252.83), (-5.084, 253.0), (-5.084, 252.83), (-5.084, 253.0), (-5.084, 252.85), (-8.801, 253.0), (-8.801, 252.85), (-0.3, 252.83), (-0.3, 252.66), (-5.084, 252.83), (-5.084, 252.66), (-5.084, 252.7), (-5.084, 252.7), (-8.801, 252.85), (-8.801, 252.7), (-0.3, 252.66), (-0.3, 252.51), (-5.084, 252.66), (-5.084, 252.55), (-5.084, 252.7), (-5.084, 252.7), (-8.801, 252.85), (-8.801, 252.7)]</t>
         </is>
       </c>
     </row>
@@ -2967,7 +2967,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>[(-0.3, 254.0), (-0.3, 253.79), (-5.837, 254.0), (-5.837, 253.79), (-5.837, 254.0), (-5.837, 253.82), (-9.608, 254.0), (-9.608, 253.82), (-0.3, 253.79), (-0.3, 253.59), (-5.837, 253.79), (-5.837, 253.64), (-5.837, 253.64), (-9.608, 253.65), (-5.837, 253.82), (-9.608, 253.65)]</t>
+          <t>[(-0.3, 254.0), (-0.3, 253.79), (-5.837, 254.0), (-5.837, 253.79), (-5.837, 254.0), (-5.837, 253.82), (-9.608, 254.0), (-9.608, 253.82), (-0.3, 253.79), (-0.3, 253.59), (-5.837, 253.79), (-5.837, 253.64), (-5.837, 253.82), (-5.837, 253.64), (-9.608, 253.82), (-9.608, 253.65)]</t>
         </is>
       </c>
     </row>
@@ -2977,7 +2977,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>[(-0.3, 255.0), (-0.3, 254.84), (-6.327, 255.0), (-6.327, 254.84), (-6.327, 255.0), (-6.327, 254.85), (-10.119, 255.0), (-10.119, 254.85), (-0.3, 254.84), (-0.3, 254.69), (-6.327, 254.84), (-6.327, 254.72), (-6.327, 254.72), (-10.119, 254.74), (-6.327, 254.85), (-10.119, 254.74)]</t>
+          <t>[(-0.3, 255.0), (-0.3, 254.84), (-6.327, 255.0), (-6.327, 254.84), (-6.327, 255.0), (-6.327, 254.85), (-10.119, 255.0), (-10.119, 254.85), (-0.3, 254.84), (-0.3, 254.69), (-6.327, 254.84), (-6.327, 254.72), (-6.327, 254.85), (-6.327, 254.72), (-10.119, 254.85), (-10.119, 254.74)]</t>
         </is>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>[(-0.3, 256.0), (-0.3, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-10.601, 256.0), (-10.601, 255.84), (-0.3, 255.84), (-0.3, 255.69), (-6.895, 255.84), (-6.895, 255.7), (-6.895, 255.7), (-10.601, 255.69), (-6.895, 255.84), (-10.601, 255.69)]</t>
+          <t>[(-0.3, 256.0), (-0.3, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-6.895, 256.0), (-6.895, 255.84), (-10.601, 256.0), (-10.601, 255.84), (-0.3, 255.84), (-0.3, 255.69), (-6.895, 255.84), (-6.895, 255.7), (-6.895, 255.84), (-6.895, 255.7), (-10.601, 255.84), (-10.601, 255.69)]</t>
         </is>
       </c>
     </row>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>[(-0.3, 257.0), (-0.3, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-11.175, 257.0), (-11.175, 256.79), (-0.3, 256.79), (-0.3, 256.59), (-7.551, 256.79), (-7.551, 256.62), (-7.551, 256.62), (-11.175, 256.59), (-7.551, 256.79), (-11.175, 256.59)]</t>
+          <t>[(-0.3, 257.0), (-0.3, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-7.551, 257.0), (-7.551, 256.79), (-11.175, 257.0), (-11.175, 256.79), (-0.3, 256.79), (-0.3, 256.59), (-7.551, 256.79), (-7.551, 256.62), (-7.551, 256.79), (-7.551, 256.62), (-11.175, 256.79), (-11.175, 256.59)]</t>
         </is>
       </c>
     </row>
@@ -3007,7 +3007,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>[(-0.3, 258.0), (-0.3, 257.78), (-8.147, 258.0), (-8.147, 257.78), (-8.147, 258.0), (-8.147, 257.82), (-11.826, 258.0), (-11.826, 257.82), (-0.3, 257.78), (-0.3, 257.57), (-8.147, 257.78), (-8.147, 257.65), (-8.147, 257.65), (-11.826, 257.69), (-8.147, 257.82), (-11.826, 257.69)]</t>
+          <t>[(-0.3, 258.0), (-0.3, 257.78), (-8.147, 258.0), (-8.147, 257.78), (-8.147, 258.0), (-8.147, 257.82), (-11.826, 258.0), (-11.826, 257.82), (-0.3, 257.78), (-0.3, 257.57), (-8.147, 257.78), (-8.147, 257.65), (-8.147, 257.82), (-8.147, 257.65), (-11.826, 257.82), (-11.826, 257.69)]</t>
         </is>
       </c>
     </row>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>[(-0.3, 259.0), (-0.3, 258.89), (-8.681, 259.0), (-8.681, 258.89), (-8.681, 259.0), (-8.681, 258.89), (-12.316, 259.0), (-12.316, 258.89), (-0.3, 258.89), (-0.3, 258.59), (-8.681, 258.89), (-8.681, 258.69), (-8.681, 258.69), (-12.316, 258.75), (-8.681, 258.89), (-12.316, 258.75)]</t>
+          <t>[(-0.3, 259.0), (-0.3, 258.89), (-8.681, 259.0), (-8.681, 258.89), (-8.681, 259.0), (-8.681, 258.89), (-12.316, 259.0), (-12.316, 258.89), (-0.3, 258.89), (-0.3, 258.59), (-8.681, 258.89), (-8.681, 258.69), (-8.681, 258.89), (-8.681, 258.69), (-12.316, 258.89), (-12.316, 258.75)]</t>
         </is>
       </c>
     </row>
@@ -3027,7 +3027,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[(-0.3, 260.0), (-0.3, 259.76), (-8.606, 260.0), (-8.606, 259.76), (-8.606, 260.0), (-8.606, 259.82), (-12.32, 260.0), (-12.32, 259.82), (-0.3, 259.76), (-0.3, 259.53), (-8.606, 259.76), (-8.606, 259.65), (-8.606, 259.65), (-12.32, 259.71), (-8.606, 259.82), (-12.32, 259.71)]</t>
+          <t>[(-0.3, 260.0), (-0.3, 259.76), (-8.606, 260.0), (-8.606, 259.76), (-8.606, 260.0), (-8.606, 259.82), (-12.32, 260.0), (-12.32, 259.82), (-0.3, 259.76), (-0.3, 259.53), (-8.606, 259.76), (-8.606, 259.65), (-8.606, 259.82), (-8.606, 259.65), (-12.32, 259.82), (-12.32, 259.71)]</t>
         </is>
       </c>
     </row>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>[(-0.3, 261.0), (-0.3, 260.71), (-8.556, 261.0), (-8.556, 260.71), (-8.556, 261.0), (-8.556, 260.8), (-12.298, 261.0), (-12.298, 260.8), (-0.3, 260.71), (-0.3, 260.42), (-8.556, 260.71), (-8.556, 260.6), (-8.556, 260.6), (-12.298, 260.65), (-8.556, 260.8), (-12.298, 260.65)]</t>
+          <t>[(-0.3, 261.0), (-0.3, 260.71), (-8.556, 261.0), (-8.556, 260.71), (-8.556, 261.0), (-8.556, 260.8), (-12.298, 261.0), (-12.298, 260.8), (-0.3, 260.71), (-0.3, 260.42), (-8.556, 260.71), (-8.556, 260.6), (-8.556, 260.8), (-8.556, 260.6), (-12.298, 260.8), (-12.298, 260.65)]</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>[(-0.3, 262.0), (-0.3, 261.67), (-8.125, 262.0), (-8.125, 262.0), (-8.125, 262.0), (-8.125, 261.83), (-12.034, 262.0), (-12.034, 261.83), (-0.3, 261.67), (-0.3, 261.34), (-8.125, 262.0), (-8.125, 261.74), (-8.125, 261.66), (-12.034, 261.66), (-8.125, 261.83), (-12.034, 261.66)]</t>
+          <t>[(-0.3, 262.0), (-0.3, 261.67), (-8.125, 262.0), (-8.125, 262.0), (-8.125, 262.0), (-8.125, 261.83), (-12.034, 262.0), (-12.034, 261.83), (-0.3, 261.67), (-0.3, 261.34), (-8.125, 262.0), (-8.125, 261.74), (-8.125, 261.83), (-8.125, 261.66), (-12.034, 261.83), (-12.034, 261.66)]</t>
         </is>
       </c>
     </row>
@@ -3057,7 +3057,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>[(-0.3, 263.0), (-0.3, 262.66), (-7.604, 263.0), (-7.604, 263.0), (-7.604, 263.0), (-7.604, 262.81), (-11.496, 263.0), (-11.496, 262.81), (-0.3, 262.66), (-0.3, 262.32), (-7.604, 263.0), (-7.604, 262.72), (-7.604, 262.62), (-11.496, 262.62), (-7.604, 262.81), (-11.496, 262.62)]</t>
+          <t>[(-0.3, 263.0), (-0.3, 262.66), (-7.604, 263.0), (-7.604, 263.0), (-7.604, 263.0), (-7.604, 262.81), (-11.496, 263.0), (-11.496, 262.81), (-0.3, 262.66), (-0.3, 262.32), (-7.604, 263.0), (-7.604, 262.72), (-7.604, 262.81), (-7.604, 262.62), (-11.496, 262.81), (-11.496, 262.62)]</t>
         </is>
       </c>
     </row>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>[(-0.3, 264.0), (-0.3, 263.7), (-6.979, 264.0), (-6.979, 263.7), (-6.979, 264.0), (-6.979, 263.84), (-10.837, 264.0), (-10.837, 263.84), (-0.3, 263.7), (-0.3, 263.41), (-6.979, 263.7), (-6.979, 263.52), (-6.979, 263.68), (-10.837, 263.68), (-6.979, 263.84), (-10.837, 263.68)]</t>
+          <t>[(-0.3, 264.0), (-0.3, 263.7), (-6.979, 264.0), (-6.979, 263.7), (-6.979, 264.0), (-6.979, 263.84), (-10.837, 264.0), (-10.837, 263.84), (-0.3, 263.7), (-0.3, 263.41), (-6.979, 263.7), (-6.979, 263.52), (-6.979, 263.84), (-6.979, 263.68), (-10.837, 263.84), (-10.837, 263.68)]</t>
         </is>
       </c>
     </row>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3087,7 +3087,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>[(-0.3, 266.0), (-0.3, 265.75), (-6.725, 266.0), (-6.725, 265.75), (-6.725, 266.0), (-6.725, 265.82), (-10.403, 266.0), (-10.403, 265.82), (-0.3, 265.75), (-0.3, 265.5), (-6.725, 265.75), (-6.725, 265.64), (-6.725, 265.64), (-10.403, 265.7), (-6.725, 265.82), (-10.403, 265.7)]</t>
+          <t>[(-0.3, 266.0), (-0.3, 265.75), (-6.725, 266.0), (-6.725, 265.75), (-6.725, 266.0), (-6.725, 265.82), (-10.403, 266.0), (-10.403, 265.82), (-0.3, 265.75), (-0.3, 265.5), (-6.725, 265.75), (-6.725, 265.64), (-6.725, 265.82), (-6.725, 265.64), (-10.403, 265.82), (-10.403, 265.7)]</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>[(-0.3, 267.0), (-0.3, 266.71), (-6.746, 267.0), (-6.746, 266.71), (-6.746, 267.0), (-6.746, 266.75), (-10.553, 267.0), (-10.553, 266.75), (-0.3, 266.71), (-0.3, 266.42), (-6.746, 266.71), (-6.746, 266.5), (-6.746, 266.5), (-10.553, 266.56), (-6.746, 266.75), (-10.553, 266.56)]</t>
+          <t>[(-0.3, 267.0), (-0.3, 266.71), (-6.746, 267.0), (-6.746, 266.71), (-6.746, 267.0), (-6.746, 266.75), (-10.553, 267.0), (-10.553, 266.75), (-0.3, 266.71), (-0.3, 266.42), (-6.746, 266.71), (-6.746, 266.5), (-6.746, 266.75), (-6.746, 266.5), (-10.553, 266.75), (-10.553, 266.56)]</t>
         </is>
       </c>
     </row>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>[(-0.3, 268.0), (-0.3, 267.8), (-6.694, 268.0), (-6.694, 267.8), (-6.694, 268.0), (-6.694, 267.83), (-10.486, 268.0), (-10.486, 267.83), (-0.3, 267.8), (-0.3, 267.6), (-6.694, 267.8), (-6.694, 267.6), (-6.694, 267.66), (-10.486, 267.66), (-6.694, 267.83), (-10.486, 267.66), (-0.3, 267.6), (-0.3, 267.4), (-6.694, 267.6), (-6.694, 267.49), (-6.694, 267.66), (-10.486, 267.66), (-6.694, 267.83), (-10.486, 267.66)]</t>
+          <t>[(-0.3, 268.0), (-0.3, 267.8), (-6.694, 268.0), (-6.694, 267.8), (-6.694, 268.0), (-6.694, 267.83), (-10.486, 268.0), (-10.486, 267.83), (-0.3, 267.8), (-0.3, 267.6), (-6.694, 267.8), (-6.694, 267.6), (-6.694, 267.66), (-6.694, 267.66), (-10.486, 267.83), (-10.486, 267.66), (-0.3, 267.6), (-0.3, 267.4), (-6.694, 267.6), (-6.694, 267.49), (-6.694, 267.66), (-6.694, 267.66), (-10.486, 267.83), (-10.486, 267.66)]</t>
         </is>
       </c>
     </row>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>[(-0.3, 269.0), (-0.3, 268.82), (-6.61, 269.0), (-6.61, 268.82), (-6.61, 269.0), (-6.61, 268.76), (-10.361, 269.0), (-10.361, 268.76), (-0.3, 268.82), (-0.3, 268.64), (-6.61, 268.82), (-6.61, 268.64), (-6.61, 268.52), (-10.361, 268.58), (-6.61, 268.76), (-10.361, 268.58), (-0.3, 268.64), (-0.3, 268.46), (-6.61, 268.64), (-6.61, 268.52), (-6.61, 268.52), (-10.361, 268.58), (-6.61, 268.76), (-10.361, 268.58)]</t>
+          <t>[(-0.3, 269.0), (-0.3, 268.82), (-6.61, 269.0), (-6.61, 268.82), (-6.61, 269.0), (-6.61, 268.76), (-10.361, 269.0), (-10.361, 268.76), (-0.3, 268.82), (-0.3, 268.64), (-6.61, 268.82), (-6.61, 268.64), (-6.61, 268.52), (-6.61, 268.58), (-10.361, 268.76), (-10.361, 268.58), (-0.3, 268.64), (-0.3, 268.46), (-6.61, 268.64), (-6.61, 268.52), (-6.61, 268.52), (-6.61, 268.52), (-10.361, 268.76), (-10.361, 268.58)]</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3127,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>[(-0.3, 270.0), (-0.3, 269.77), (-5.972, 270.0), (-5.972, 269.77), (-5.972, 270.0), (-5.972, 269.8), (-9.945, 270.0), (-9.945, 269.8), (-0.3, 269.77), (-0.3, 269.55), (-5.972, 269.77), (-5.972, 269.61), (-5.972, 269.61), (-9.945, 269.67), (-5.972, 269.8), (-9.945, 269.67)]</t>
+          <t>[(-0.3, 270.0), (-0.3, 269.77), (-5.972, 270.0), (-5.972, 269.77), (-5.972, 270.0), (-5.972, 269.8), (-9.945, 270.0), (-9.945, 269.8), (-0.3, 269.77), (-0.3, 269.55), (-5.972, 269.77), (-5.972, 269.61), (-5.972, 269.8), (-5.972, 269.61), (-9.945, 269.8), (-9.945, 269.67)]</t>
         </is>
       </c>
     </row>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>[(-0.3, 271.0), (-0.3, 270.8), (-5.101, 271.0), (-5.101, 270.8), (-5.101, 271.0), (-5.101, 270.82), (-8.92, 271.0), (-8.92, 270.82), (-0.3, 270.8), (-0.3, 270.6), (-5.101, 270.8), (-5.101, 270.65), (-5.101, 270.65), (-8.92, 270.71), (-5.101, 270.82), (-8.92, 270.71)]</t>
+          <t>[(-0.3, 271.0), (-0.3, 270.8), (-5.101, 271.0), (-5.101, 270.8), (-5.101, 271.0), (-5.101, 270.82), (-8.92, 271.0), (-8.92, 270.82), (-0.3, 270.8), (-0.3, 270.6), (-5.101, 270.8), (-5.101, 270.65), (-5.101, 270.82), (-5.101, 270.65), (-8.92, 270.82), (-8.92, 270.71)]</t>
         </is>
       </c>
     </row>
@@ -3147,7 +3147,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>[(-0.3, 272.0), (-0.3, 271.8), (-4.282, 272.0), (-4.282, 271.8), (-4.282, 272.0), (-4.282, 271.89), (-7.976, 272.0), (-7.976, 271.89), (-0.3, 271.8), (-0.3, 271.61), (-4.282, 271.8), (-4.282, 271.68), (-4.282, 271.68), (-7.976, 271.74), (-4.282, 271.89), (-7.976, 271.74)]</t>
+          <t>[(-0.3, 272.0), (-0.3, 271.8), (-4.282, 272.0), (-4.282, 271.8), (-4.282, 272.0), (-4.282, 271.89), (-7.976, 272.0), (-7.976, 271.89), (-0.3, 271.8), (-0.3, 271.61), (-4.282, 271.8), (-4.282, 271.68), (-4.282, 271.89), (-4.282, 271.68), (-7.976, 271.89), (-7.976, 271.74)]</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3157,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>[(-0.3, 273.0), (-0.3, 272.83), (-3.183, 273.0), (-3.183, 272.83), (-3.183, 273.0), (-3.183, 272.85), (-6.948, 273.0), (-6.948, 272.85), (-0.3, 272.83), (-0.3, 272.66), (-3.183, 272.83), (-3.183, 272.7), (-3.183, 272.7), (-6.948, 272.73), (-3.183, 272.85), (-6.948, 272.73)]</t>
+          <t>[(-0.3, 273.0), (-0.3, 272.83), (-3.183, 273.0), (-3.183, 272.83), (-3.183, 273.0), (-3.183, 272.85), (-6.948, 273.0), (-6.948, 272.85), (-0.3, 272.83), (-0.3, 272.66), (-3.183, 272.83), (-3.183, 272.7), (-3.183, 272.85), (-3.183, 272.7), (-6.948, 272.85), (-6.948, 272.73)]</t>
         </is>
       </c>
     </row>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3247,7 +3247,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3267,7 +3267,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3287,7 +3287,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3307,7 +3307,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3317,7 +3317,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3327,7 +3327,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3347,7 +3347,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3507,7 +3507,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3527,7 +3527,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3547,7 +3547,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3567,7 +3567,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3577,7 +3577,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3587,7 +3587,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3607,7 +3607,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3627,7 +3627,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3647,7 +3647,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3667,7 +3667,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3687,7 +3687,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3697,7 +3697,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3707,7 +3707,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3747,7 +3747,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3767,7 +3767,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3777,7 +3777,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3787,7 +3787,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3797,7 +3797,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3817,7 +3817,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3827,7 +3827,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3847,7 +3847,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3867,7 +3867,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3877,7 +3877,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3887,7 +3887,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3907,7 +3907,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3937,7 +3937,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3947,7 +3947,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3967,7 +3967,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4007,7 +4007,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4017,7 +4017,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4037,7 +4037,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4047,7 +4047,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4067,7 +4067,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4087,7 +4087,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4097,7 +4097,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4107,7 +4107,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4117,7 +4117,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4127,7 +4127,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4147,7 +4147,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4157,7 +4157,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4167,7 +4167,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4177,7 +4177,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4187,7 +4187,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4197,7 +4197,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4257,7 +4257,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4267,7 +4267,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4277,7 +4277,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4287,7 +4287,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4297,7 +4297,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4307,7 +4307,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4317,7 +4317,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4327,7 +4327,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4337,7 +4337,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4347,7 +4347,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4357,7 +4357,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4367,7 +4367,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4377,7 +4377,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4397,7 +4397,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4407,7 +4407,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4417,7 +4417,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4427,7 +4427,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4447,7 +4447,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4457,7 +4457,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4467,7 +4467,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4477,7 +4477,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4487,7 +4487,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4497,7 +4497,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4507,7 +4507,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4517,7 +4517,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4527,7 +4527,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4537,7 +4537,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4547,7 +4547,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4557,7 +4557,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4567,7 +4567,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4577,7 +4577,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4587,7 +4587,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4597,7 +4597,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4607,7 +4607,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4617,7 +4617,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4627,7 +4627,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4637,7 +4637,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4647,7 +4647,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4657,7 +4657,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4667,7 +4667,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4687,7 +4687,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4707,7 +4707,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4717,7 +4717,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4727,7 +4727,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4737,7 +4737,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4747,7 +4747,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4757,7 +4757,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4767,7 +4767,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4787,7 +4787,7 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4797,7 +4797,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -4807,7 +4807,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5017,7 +5017,7 @@
       </c>
       <c r="B460" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5047,7 +5047,7 @@
       </c>
       <c r="B463" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="B464" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="B465" t="inlineStr">
         <is>
-          <t>[(-0.3, 464.0), (-0.3, 463.85), (-2.353, 464.0), (-2.353, 463.85), (-2.353, 464.0), (-2.353, 463.89), (-9.118, 464.0), (-9.118, 463.89), (-0.3, 463.85), (-0.3, 463.74), (-2.353, 463.85), (-2.353, 463.72), (-2.353, 463.72), (-9.118, 463.62), (-2.353, 463.89), (-9.118, 463.62)]</t>
+          <t>[(-0.3, 464.0), (-0.3, 463.85), (-2.353, 464.0), (-2.353, 463.85), (-2.353, 464.0), (-2.353, 463.89), (-9.118, 464.0), (-9.118, 463.89), (-0.3, 463.85), (-0.3, 463.74), (-2.353, 463.85), (-2.353, 463.72), (-2.353, 463.89), (-2.353, 463.72), (-9.118, 463.89), (-9.118, 463.62)]</t>
         </is>
       </c>
     </row>
@@ -5077,7 +5077,7 @@
       </c>
       <c r="B466" t="inlineStr">
         <is>
-          <t>[(-0.3, 465.0), (-0.3, 464.85), (-2.525, 465.0), (-2.525, 464.85), (-2.525, 465.0), (-2.525, 464.87), (-9.207, 465.0), (-9.207, 464.87), (-0.3, 464.85), (-0.3, 464.74), (-2.525, 464.85), (-2.525, 464.72), (-2.525, 464.72), (-9.207, 464.57), (-2.525, 464.87), (-9.207, 464.57)]</t>
+          <t>[(-0.3, 465.0), (-0.3, 464.85), (-2.525, 465.0), (-2.525, 464.85), (-2.525, 465.0), (-2.525, 464.87), (-9.207, 465.0), (-9.207, 464.87), (-0.3, 464.85), (-0.3, 464.74), (-2.525, 464.85), (-2.525, 464.72), (-2.525, 464.87), (-2.525, 464.72), (-9.207, 464.87), (-9.207, 464.57)]</t>
         </is>
       </c>
     </row>
@@ -5087,7 +5087,7 @@
       </c>
       <c r="B467" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5097,7 +5097,7 @@
       </c>
       <c r="B468" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5107,7 +5107,7 @@
       </c>
       <c r="B469" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5117,7 +5117,7 @@
       </c>
       <c r="B470" t="inlineStr">
         <is>
-          <t>[(-0.3, 469.0), (-0.3, 468.84), (-3.597, 469.0), (-3.597, 468.84), (-3.597, 469.0), (-3.597, 468.86), (-10.382, 469.0), (-10.382, 468.86), (-0.3, 468.84), (-0.3, 468.72), (-3.597, 468.84), (-3.597, 468.68), (-3.597, 468.68), (-10.382, 468.56), (-3.597, 468.86), (-10.382, 468.56)]</t>
+          <t>[(-0.3, 469.0), (-0.3, 468.84), (-3.597, 469.0), (-3.597, 468.84), (-3.597, 469.0), (-3.597, 468.86), (-10.382, 469.0), (-10.382, 468.86), (-0.3, 468.84), (-0.3, 468.72), (-3.597, 468.84), (-3.597, 468.68), (-3.597, 468.86), (-3.597, 468.68), (-10.382, 468.86), (-10.382, 468.56)]</t>
         </is>
       </c>
     </row>
@@ -5127,7 +5127,7 @@
       </c>
       <c r="B471" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B472" t="inlineStr">
         <is>
-          <t>[(-0.3, 471.0), (-0.3, 470.84), (-4.191, 471.0), (-4.191, 470.84), (-4.191, 471.0), (-4.191, 470.85), (-10.943, 471.0), (-10.943, 470.85), (-0.3, 470.84), (-0.3, 470.72), (-4.191, 470.84), (-4.191, 470.69), (-4.191, 470.69), (-10.943, 470.55), (-4.191, 470.85), (-10.943, 470.55)]</t>
+          <t>[(-0.3, 471.0), (-0.3, 470.84), (-4.191, 471.0), (-4.191, 470.84), (-4.191, 471.0), (-4.191, 470.85), (-10.943, 471.0), (-10.943, 470.85), (-0.3, 470.84), (-0.3, 470.72), (-4.191, 470.84), (-4.191, 470.69), (-4.191, 470.85), (-4.191, 470.69), (-10.943, 470.85), (-10.943, 470.55)]</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="B473" t="inlineStr">
         <is>
-          <t>[(-0.3, 472.0), (-0.3, 471.86), (-4.416, 472.0), (-4.416, 471.86), (-4.416, 472.0), (-4.416, 471.85), (-11.157, 472.0), (-11.157, 471.85), (-0.3, 471.86), (-0.3, 471.74), (-4.416, 471.86), (-4.416, 471.73), (-4.416, 471.73), (-11.157, 471.55), (-4.416, 471.85), (-11.157, 471.55)]</t>
+          <t>[(-0.3, 472.0), (-0.3, 471.86), (-4.416, 472.0), (-4.416, 471.86), (-4.416, 472.0), (-4.416, 471.85), (-11.157, 472.0), (-11.157, 471.85), (-0.3, 471.86), (-0.3, 471.74), (-4.416, 471.86), (-4.416, 471.73), (-4.416, 471.85), (-4.416, 471.73), (-11.157, 471.85), (-11.157, 471.55)]</t>
         </is>
       </c>
     </row>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="B474" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5167,7 +5167,7 @@
       </c>
       <c r="B475" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="B476" t="inlineStr">
         <is>
-          <t>[(-0.3, 475.0), (-0.3, 474.85), (-4.821, 475.0), (-4.821, 474.85), (-4.821, 475.0), (-4.821, 474.86), (-11.595, 475.0), (-11.595, 474.86), (-0.3, 474.85), (-0.3, 474.74), (-4.821, 474.85), (-4.821, 474.71), (-4.821, 474.71), (-11.595, 474.56), (-4.821, 474.86), (-11.595, 474.56)]</t>
+          <t>[(-0.3, 475.0), (-0.3, 474.85), (-4.821, 475.0), (-4.821, 474.85), (-4.821, 475.0), (-4.821, 474.86), (-11.595, 475.0), (-11.595, 474.86), (-0.3, 474.85), (-0.3, 474.74), (-4.821, 474.85), (-4.821, 474.71), (-4.821, 474.86), (-4.821, 474.71), (-11.595, 474.86), (-11.595, 474.56)]</t>
         </is>
       </c>
     </row>
@@ -5187,7 +5187,7 @@
       </c>
       <c r="B477" t="inlineStr">
         <is>
-          <t>[(-0.3, 476.0), (-0.3, 475.85), (-4.916, 476.0), (-4.916, 475.85), (-4.916, 476.0), (-4.916, 475.89), (-11.628, 476.0), (-11.628, 475.89), (-0.3, 475.85), (-0.3, 475.74), (-4.916, 475.85), (-4.916, 475.71), (-4.916, 475.71), (-11.628, 475.59), (-4.916, 475.89), (-11.628, 475.59)]</t>
+          <t>[(-0.3, 476.0), (-0.3, 475.85), (-4.916, 476.0), (-4.916, 475.85), (-4.916, 476.0), (-4.916, 475.89), (-11.628, 476.0), (-11.628, 475.89), (-0.3, 475.85), (-0.3, 475.74), (-4.916, 475.85), (-4.916, 475.71), (-4.916, 475.89), (-4.916, 475.71), (-11.628, 475.89), (-11.628, 475.59)]</t>
         </is>
       </c>
     </row>
@@ -5197,7 +5197,7 @@
       </c>
       <c r="B478" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5207,7 +5207,7 @@
       </c>
       <c r="B479" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5217,7 @@
       </c>
       <c r="B480" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5227,7 +5227,7 @@
       </c>
       <c r="B481" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5237,7 +5237,7 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>[(-0.3, 482.0), (-0.3, 481.84), (-4.711, 482.0), (-4.711, 481.84), (-4.711, 482.0), (-4.711, 481.81), (-11.456, 482.0), (-11.456, 481.81), (-0.3, 481.84), (-0.3, 481.73), (-4.711, 481.84), (-4.711, 481.69), (-4.711, 481.69), (-11.456, 481.51), (-4.711, 481.81), (-11.456, 481.51)]</t>
+          <t>[(-0.3, 482.0), (-0.3, 481.84), (-4.711, 482.0), (-4.711, 481.84), (-4.711, 482.0), (-4.711, 481.81), (-11.456, 482.0), (-11.456, 481.81), (-0.3, 481.84), (-0.3, 481.73), (-4.711, 481.84), (-4.711, 481.69), (-4.711, 481.81), (-4.711, 481.69), (-11.456, 481.81), (-11.456, 481.51)]</t>
         </is>
       </c>
     </row>
@@ -5257,7 +5257,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>[(-0.3, 483.0), (-0.3, 482.83), (-4.708, 483.0), (-4.708, 482.83), (-4.708, 483.0), (-4.708, 482.81), (-11.451, 483.0), (-11.451, 482.81), (-0.3, 482.83), (-0.3, 482.71), (-4.708, 482.83), (-4.708, 482.67), (-4.708, 482.67), (-11.451, 482.51), (-4.708, 482.81), (-11.451, 482.51)]</t>
+          <t>[(-0.3, 483.0), (-0.3, 482.83), (-4.708, 483.0), (-4.708, 482.83), (-4.708, 483.0), (-4.708, 482.81), (-11.451, 483.0), (-11.451, 482.81), (-0.3, 482.83), (-0.3, 482.71), (-4.708, 482.83), (-4.708, 482.67), (-4.708, 482.81), (-4.708, 482.67), (-11.451, 482.81), (-11.451, 482.51)]</t>
         </is>
       </c>
     </row>
@@ -5267,7 +5267,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>[(-0.3, 484.0), (-0.3, 483.82), (-4.827, 484.0), (-4.827, 483.82), (-4.827, 484.0), (-4.827, 483.75), (-11.636, 484.0), (-11.636, 483.75), (-0.3, 483.82), (-0.3, 483.69), (-4.827, 483.82), (-4.827, 483.64), (-4.827, 483.64), (-11.636, 483.51), (-4.827, 483.75), (-11.636, 483.51)]</t>
+          <t>[(-0.3, 484.0), (-0.3, 483.82), (-4.827, 484.0), (-4.827, 483.82), (-4.827, 484.0), (-4.827, 483.75), (-11.636, 484.0), (-11.636, 483.75), (-0.3, 483.82), (-0.3, 483.69), (-4.827, 483.82), (-4.827, 483.64), (-4.827, 483.75), (-4.827, 483.64), (-11.636, 483.75), (-11.636, 483.51)]</t>
         </is>
       </c>
     </row>
@@ -5277,7 +5277,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>[(-0.3, 485.0), (-0.3, 484.82), (-5.008, 485.0), (-5.008, 484.82), (-5.008, 485.0), (-5.008, 484.78), (-11.805, 485.0), (-11.805, 484.78), (-0.3, 484.82), (-0.3, 484.67), (-5.008, 484.82), (-5.008, 484.65), (-5.008, 484.65), (-11.805, 484.57), (-5.008, 484.78), (-11.805, 484.57)]</t>
+          <t>[(-0.3, 485.0), (-0.3, 484.82), (-5.008, 485.0), (-5.008, 484.82), (-5.008, 485.0), (-5.008, 484.78), (-11.805, 485.0), (-11.805, 484.78), (-0.3, 484.82), (-0.3, 484.67), (-5.008, 484.82), (-5.008, 484.65), (-5.008, 484.78), (-5.008, 484.65), (-11.805, 484.78), (-11.805, 484.57)]</t>
         </is>
       </c>
     </row>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>[(-0.3, 486.0), (-0.3, 485.85), (-5.129, 486.0), (-5.129, 485.85), (-5.129, 486.0), (-5.129, 485.73), (-12.005, 486.0), (-12.005, 485.73), (-0.3, 485.85), (-0.3, 485.7), (-5.129, 485.85), (-5.129, 485.7), (-5.129, 485.58), (-12.005, 485.46), (-5.129, 485.73), (-12.005, 485.46), (-0.3, 485.7), (-0.3, 485.58), (-5.129, 485.7), (-5.129, 485.58), (-5.129, 485.58), (-12.005, 485.46), (-5.129, 485.73), (-12.005, 485.46)]</t>
+          <t>[(-0.3, 486.0), (-0.3, 485.85), (-5.129, 486.0), (-5.129, 485.85), (-5.129, 486.0), (-5.129, 485.73), (-12.005, 486.0), (-12.005, 485.73), (-0.3, 485.85), (-0.3, 485.7), (-5.129, 485.85), (-5.129, 485.7), (-5.129, 485.58), (-5.129, 485.46), (-12.005, 485.73), (-12.005, 485.46), (-0.3, 485.7), (-0.3, 485.58), (-5.129, 485.7), (-5.129, 485.58), (-5.129, 485.58), (-5.129, 485.58), (-12.005, 485.73), (-12.005, 485.46)]</t>
         </is>
       </c>
     </row>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>[(-0.3, 487.0), (-0.3, 486.82), (-5.221, 487.0), (-5.221, 486.82), (-5.221, 487.0), (-5.221, 486.81), (-11.995, 487.0), (-11.995, 486.81), (-0.3, 486.82), (-0.3, 486.64), (-5.221, 486.82), (-5.221, 486.64), (-5.221, 486.62), (-11.995, 486.62), (-5.221, 486.81), (-11.995, 486.62), (-0.3, 486.64), (-0.3, 486.48), (-5.221, 486.64), (-5.221, 486.5), (-5.221, 486.62), (-11.995, 486.62), (-5.221, 486.81), (-11.995, 486.62)]</t>
+          <t>[(-0.3, 487.0), (-0.3, 486.82), (-5.221, 487.0), (-5.221, 486.82), (-5.221, 487.0), (-5.221, 486.81), (-11.995, 487.0), (-11.995, 486.81), (-0.3, 486.82), (-0.3, 486.64), (-5.221, 486.82), (-5.221, 486.64), (-5.221, 486.62), (-5.221, 486.62), (-11.995, 486.81), (-11.995, 486.62), (-0.3, 486.64), (-0.3, 486.48), (-5.221, 486.64), (-5.221, 486.5), (-5.221, 486.62), (-5.221, 486.62), (-11.995, 486.81), (-11.995, 486.62)]</t>
         </is>
       </c>
     </row>
@@ -5307,7 +5307,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>[(-0.3, 488.0), (-0.3, 487.7), (-5.246, 488.0), (-5.246, 487.7), (-5.246, 488.0), (-5.246, 487.83), (-12.042, 488.0), (-12.042, 487.83), (-0.3, 487.7), (-0.3, 487.41), (-5.246, 487.7), (-5.246, 487.52), (-5.246, 487.66), (-12.042, 487.66), (-5.246, 487.83), (-12.042, 487.66)]</t>
+          <t>[(-0.3, 488.0), (-0.3, 487.7), (-5.246, 488.0), (-5.246, 487.7), (-5.246, 488.0), (-5.246, 487.83), (-12.042, 488.0), (-12.042, 487.83), (-0.3, 487.7), (-0.3, 487.41), (-5.246, 487.7), (-5.246, 487.52), (-5.246, 487.83), (-5.246, 487.66), (-12.042, 487.83), (-12.042, 487.66)]</t>
         </is>
       </c>
     </row>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>[(-0.3, 489.0), (-0.3, 488.73), (-5.258, 489.0), (-5.258, 488.73), (-5.258, 489.0), (-5.258, 488.89), (-12.017, 489.0), (-12.017, 488.89), (-0.3, 488.73), (-0.3, 488.43), (-5.258, 488.73), (-5.258, 488.61), (-5.258, 488.61), (-12.017, 488.74), (-5.258, 488.89), (-12.017, 488.74)]</t>
+          <t>[(-0.3, 489.0), (-0.3, 488.73), (-5.258, 489.0), (-5.258, 488.73), (-5.258, 489.0), (-5.258, 488.89), (-12.017, 489.0), (-12.017, 488.89), (-0.3, 488.73), (-0.3, 488.43), (-5.258, 488.73), (-5.258, 488.61), (-5.258, 488.89), (-5.258, 488.61), (-12.017, 488.89), (-12.017, 488.74)]</t>
         </is>
       </c>
     </row>
@@ -5327,7 +5327,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5337,7 +5337,7 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 491.0), (-5.197, 491.0), (-5.197, 491.0), (-5.197, 490.85), (-12.024, 491.0), (-12.024, 490.85), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 491.0), (-5.197, 490.78), (-5.197, 490.55), (-12.024, 490.68), (-5.197, 490.85), (-12.024, 490.68)]</t>
+          <t>[(-0.3, 491.0), (-0.3, 490.66), (-5.197, 491.0), (-5.197, 491.0), (-5.197, 491.0), (-5.197, 490.85), (-12.024, 491.0), (-12.024, 490.85), (-0.3, 490.66), (-0.3, 490.32), (-5.197, 491.0), (-5.197, 490.78), (-5.197, 490.85), (-5.197, 490.55), (-12.024, 490.85), (-12.024, 490.68)]</t>
         </is>
       </c>
     </row>
@@ -5347,7 +5347,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 492.0), (-5.221, 492.0), (-5.221, 492.0), (-5.221, 491.72), (-12.004, 492.0), (-12.004, 491.72), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 492.0), (-5.221, 491.72), (-5.221, 491.45), (-12.004, 491.56), (-5.221, 491.72), (-12.004, 491.56)]</t>
+          <t>[(-0.3, 492.0), (-0.3, 491.61), (-5.221, 492.0), (-5.221, 492.0), (-5.221, 492.0), (-5.221, 491.72), (-12.004, 492.0), (-12.004, 491.72), (-0.3, 491.61), (-0.3, 491.22), (-5.221, 492.0), (-5.221, 491.72), (-5.221, 491.72), (-5.221, 491.45), (-12.004, 491.72), (-12.004, 491.56)]</t>
         </is>
       </c>
     </row>
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 493.0), (-5.159, 493.0), (-5.159, 493.0), (-5.159, 492.79), (-11.984, 493.0), (-11.984, 492.79), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 493.0), (-5.159, 492.68), (-5.159, 492.58), (-11.984, 492.58), (-5.159, 492.79), (-11.984, 492.58)]</t>
+          <t>[(-0.3, 493.0), (-0.3, 492.55), (-5.159, 493.0), (-5.159, 493.0), (-5.159, 493.0), (-5.159, 492.79), (-11.984, 493.0), (-11.984, 492.79), (-0.3, 492.55), (-0.3, 492.1), (-5.159, 493.0), (-5.159, 492.68), (-5.159, 492.79), (-5.159, 492.58), (-11.984, 492.79), (-11.984, 492.58)]</t>
         </is>
       </c>
     </row>
@@ -5367,7 +5367,7 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 494.0), (-5.114, 494.0), (-5.114, 494.0), (-5.114, 493.73), (-11.935, 494.0), (-11.935, 493.73), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 494.0), (-5.114, 493.6), (-5.114, 493.46), (-11.935, 493.46), (-5.114, 493.73), (-11.935, 493.46)]</t>
+          <t>[(-0.3, 494.0), (-0.3, 493.5), (-5.114, 494.0), (-5.114, 494.0), (-5.114, 494.0), (-5.114, 493.73), (-11.935, 494.0), (-11.935, 493.73), (-0.3, 493.5), (-0.3, 493.0), (-5.114, 494.0), (-5.114, 493.6), (-5.114, 493.73), (-5.114, 493.46), (-11.935, 493.73), (-11.935, 493.46)]</t>
         </is>
       </c>
     </row>
@@ -5377,7 +5377,7 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 495.0), (-5.078, 495.0), (-5.078, 495.0), (-5.078, 494.79), (-11.886, 495.0), (-11.886, 494.79), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 495.0), (-5.078, 494.58), (-5.078, 494.58), (-11.886, 494.58), (-5.078, 494.79), (-11.886, 494.58)]</t>
+          <t>[(-0.3, 495.0), (-0.3, 494.5), (-5.078, 495.0), (-5.078, 495.0), (-5.078, 495.0), (-5.078, 494.79), (-11.886, 495.0), (-11.886, 494.79), (-0.3, 494.5), (-0.3, 494.0), (-5.078, 495.0), (-5.078, 494.58), (-5.078, 494.79), (-5.078, 494.58), (-11.886, 494.79), (-11.886, 494.58)]</t>
         </is>
       </c>
     </row>
@@ -5387,7 +5387,7 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5407,7 +5407,7 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 499.0), (-5.357, 498.71), (-5.357, 499.0), (-5.357, 498.76), (-12.301, 499.0), (-12.301, 498.76), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.71), (-5.357, 498.42), (-5.357, 498.52), (-12.301, 498.52), (-5.357, 498.76), (-12.301, 498.52), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.42), (-5.357, 498.28), (-5.357, 498.52), (-12.301, 498.52), (-5.357, 498.76), (-12.301, 498.52)]</t>
+          <t>[(-0.3, 499.0), (-0.3, 498.71), (-5.357, 499.0), (-5.357, 498.71), (-5.357, 499.0), (-5.357, 498.76), (-12.301, 499.0), (-12.301, 498.76), (-0.3, 498.71), (-0.3, 498.42), (-5.357, 498.71), (-5.357, 498.42), (-5.357, 498.52), (-5.357, 498.52), (-12.301, 498.76), (-12.301, 498.52), (-0.3, 498.42), (-0.3, 498.14), (-5.357, 498.42), (-5.357, 498.28), (-5.357, 498.52), (-5.357, 498.52), (-12.301, 498.76), (-12.301, 498.52)]</t>
         </is>
       </c>
     </row>
@@ -5427,7 +5427,7 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 500.0), (-5.533, 499.72), (-5.533, 500.0), (-5.533, 499.66), (-12.507, 500.0), (-12.507, 499.76), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.72), (-5.533, 499.44), (-5.533, 499.32), (-12.507, 499.52), (-5.533, 499.66), (-12.507, 499.52), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.44), (-5.533, 499.33), (-5.533, 499.32), (-12.507, 499.52), (-5.533, 499.66), (-12.507, 499.52)]</t>
+          <t>[(-0.3, 500.0), (-0.3, 499.72), (-5.533, 500.0), (-5.533, 499.72), (-5.533, 500.0), (-5.533, 499.66), (-12.507, 500.0), (-12.507, 499.76), (-0.3, 499.72), (-0.3, 499.44), (-5.533, 499.72), (-5.533, 499.44), (-5.533, 499.32), (-5.533, 499.52), (-12.507, 499.66), (-12.507, 499.52), (-0.3, 499.44), (-0.3, 499.17), (-5.533, 499.44), (-5.533, 499.33), (-5.533, 499.32), (-5.533, 499.32), (-12.507, 499.76), (-12.507, 499.52)]</t>
         </is>
       </c>
     </row>
@@ -5437,7 +5437,7 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 501.0), (-5.774, 501.0), (-5.774, 501.0), (-5.774, 500.7), (-12.784, 501.0), (-12.784, 500.7), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 501.0), (-5.774, 500.7), (-5.774, 500.41), (-12.784, 500.59), (-5.774, 500.7), (-12.784, 500.59)]</t>
+          <t>[(-0.3, 501.0), (-0.3, 500.6), (-5.774, 501.0), (-5.774, 501.0), (-5.774, 501.0), (-5.774, 500.7), (-12.784, 501.0), (-12.784, 500.7), (-0.3, 500.6), (-0.3, 500.2), (-5.774, 501.0), (-5.774, 500.7), (-5.774, 500.7), (-5.774, 500.41), (-12.784, 500.7), (-12.784, 500.59)]</t>
         </is>
       </c>
     </row>
@@ -5447,7 +5447,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 502.0), (-5.857, 502.0), (-5.857, 502.0), (-5.857, 501.77), (-12.779, 502.0), (-12.779, 501.87), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 502.0), (-5.857, 501.77), (-5.857, 501.54), (-12.779, 501.74), (-5.857, 501.77), (-12.779, 501.74)]</t>
+          <t>[(-0.3, 502.0), (-0.3, 501.65), (-5.857, 502.0), (-5.857, 502.0), (-5.857, 502.0), (-5.857, 501.77), (-12.779, 502.0), (-12.779, 501.87), (-0.3, 501.65), (-0.3, 501.3), (-5.857, 502.0), (-5.857, 501.77), (-5.857, 501.77), (-5.857, 501.54), (-12.779, 501.87), (-12.779, 501.74)]</t>
         </is>
       </c>
     </row>
@@ -5457,7 +5457,7 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 503.0), (-5.904, 503.0), (-5.904, 503.0), (-5.904, 502.77), (-12.805, 503.0), (-12.805, 502.87), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 503.0), (-5.904, 502.77), (-5.904, 502.54), (-12.805, 502.74), (-5.904, 502.77), (-12.805, 502.74)]</t>
+          <t>[(-0.3, 503.0), (-0.3, 502.68), (-5.904, 503.0), (-5.904, 503.0), (-5.904, 503.0), (-5.904, 502.77), (-12.805, 503.0), (-12.805, 502.87), (-0.3, 502.68), (-0.3, 502.36), (-5.904, 503.0), (-5.904, 502.77), (-5.904, 502.77), (-5.904, 502.54), (-12.805, 502.87), (-12.805, 502.74)]</t>
         </is>
       </c>
     </row>
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 504.0), (-5.981, 504.0), (-5.981, 504.0), (-5.981, 503.81), (-12.864, 504.0), (-12.864, 503.81), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 504.0), (-5.981, 503.76), (-5.981, 503.51), (-12.864, 503.65), (-5.981, 503.81), (-12.864, 503.65)]</t>
+          <t>[(-0.3, 504.0), (-0.3, 503.64), (-5.981, 504.0), (-5.981, 504.0), (-5.981, 504.0), (-5.981, 503.81), (-12.864, 504.0), (-12.864, 503.81), (-0.3, 503.64), (-0.3, 503.28), (-5.981, 504.0), (-5.981, 503.76), (-5.981, 503.81), (-5.981, 503.51), (-12.864, 503.81), (-12.864, 503.65)]</t>
         </is>
       </c>
     </row>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 505.0), (-5.857, 505.0), (-5.857, 505.0), (-5.857, 504.74), (-12.727, 505.0), (-12.727, 504.84), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 505.0), (-5.857, 504.74), (-5.857, 504.48), (-12.727, 504.68), (-5.857, 504.74), (-12.727, 504.68)]</t>
+          <t>[(-0.3, 505.0), (-0.3, 504.66), (-5.857, 505.0), (-5.857, 505.0), (-5.857, 505.0), (-5.857, 504.74), (-12.727, 505.0), (-12.727, 504.84), (-0.3, 504.66), (-0.3, 504.32), (-5.857, 505.0), (-5.857, 504.74), (-5.857, 504.74), (-5.857, 504.48), (-12.727, 504.84), (-12.727, 504.68)]</t>
         </is>
       </c>
     </row>
@@ -5487,7 +5487,7 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5497,7 +5497,7 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5507,7 +5507,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5517,7 +5517,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5527,7 +5527,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5537,7 +5537,7 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 512.0), (-4.393, 511.89), (-4.393, 512.0), (-4.393, 511.85), (-11.313, 512.0), (-11.313, 511.85), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.89), (-4.393, 511.72), (-4.393, 511.72), (-11.313, 511.55), (-4.393, 511.85), (-11.313, 511.55)]</t>
+          <t>[(-0.3, 512.0), (-0.3, 511.89), (-4.393, 512.0), (-4.393, 511.89), (-4.393, 512.0), (-4.393, 511.85), (-11.313, 512.0), (-11.313, 511.85), (-0.3, 511.89), (-0.3, 511.63), (-4.393, 511.89), (-4.393, 511.72), (-4.393, 511.85), (-4.393, 511.72), (-11.313, 511.85), (-11.313, 511.55)]</t>
         </is>
       </c>
     </row>
@@ -5557,7 +5557,7 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 513.0), (-4.237, 512.76), (-4.237, 513.0), (-4.237, 512.8), (-11.169, 513.0), (-11.169, 512.7), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.76), (-4.237, 512.59), (-4.237, 512.6), (-11.169, 512.4), (-4.237, 512.8), (-11.169, 512.4)]</t>
+          <t>[(-0.3, 513.0), (-0.3, 512.76), (-4.237, 513.0), (-4.237, 512.76), (-4.237, 513.0), (-4.237, 512.8), (-11.169, 513.0), (-11.169, 512.7), (-0.3, 512.76), (-0.3, 512.52), (-4.237, 512.76), (-4.237, 512.59), (-4.237, 512.8), (-4.237, 512.6), (-11.169, 512.7), (-11.169, 512.4)]</t>
         </is>
       </c>
     </row>
@@ -5567,7 +5567,7 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>[(-0.3, 514.0), (-0.3, 513.83), (-4.16, 514.0), (-4.16, 513.83), (-4.16, 514.0), (-4.16, 513.78), (-11.078, 514.0), (-11.078, 513.68), (-0.3, 513.83), (-0.3, 513.66), (-4.16, 513.83), (-4.16, 513.66), (-4.16, 513.56), (-11.078, 513.36), (-4.16, 513.78), (-11.078, 513.36), (-0.3, 513.66), (-0.3, 513.49), (-4.16, 513.66), (-4.16, 513.55), (-4.16, 513.56), (-11.078, 513.36), (-4.16, 513.78), (-11.078, 513.36)]</t>
+          <t>[(-0.3, 514.0), (-0.3, 513.83), (-4.16, 514.0), (-4.16, 513.83), (-4.16, 514.0), (-4.16, 513.78), (-11.078, 514.0), (-11.078, 513.68), (-0.3, 513.83), (-0.3, 513.66), (-4.16, 513.83), (-4.16, 513.66), (-4.16, 513.56), (-4.16, 513.36), (-11.078, 513.78), (-11.078, 513.36), (-0.3, 513.66), (-0.3, 513.49), (-4.16, 513.66), (-4.16, 513.55), (-4.16, 513.56), (-4.16, 513.56), (-11.078, 513.68), (-11.078, 513.36)]</t>
         </is>
       </c>
     </row>
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>[(-0.3, 515.0), (-0.3, 514.86), (-4.027, 515.0), (-4.027, 514.86), (-4.027, 515.0), (-4.027, 514.73), (-10.92, 515.0), (-10.92, 514.73), (-0.3, 514.86), (-0.3, 514.72), (-4.027, 514.86), (-4.027, 514.72), (-4.027, 514.59), (-10.92, 514.47), (-4.027, 514.73), (-10.92, 514.47), (-0.3, 514.72), (-0.3, 514.6), (-4.027, 514.72), (-4.027, 514.59), (-4.027, 514.59), (-10.92, 514.47), (-4.027, 514.73), (-10.92, 514.47)]</t>
+          <t>[(-0.3, 515.0), (-0.3, 514.86), (-4.027, 515.0), (-4.027, 514.86), (-4.027, 515.0), (-4.027, 514.73), (-10.92, 515.0), (-10.92, 514.73), (-0.3, 514.86), (-0.3, 514.72), (-4.027, 514.86), (-4.027, 514.72), (-4.027, 514.59), (-4.027, 514.47), (-10.92, 514.73), (-10.92, 514.47), (-0.3, 514.72), (-0.3, 514.6), (-4.027, 514.72), (-4.027, 514.59), (-4.027, 514.59), (-4.027, 514.59), (-10.92, 514.73), (-10.92, 514.47)]</t>
         </is>
       </c>
     </row>
@@ -5587,7 +5587,7 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>[(-0.3, 516.0), (-0.3, 515.87), (-3.916, 516.0), (-3.916, 515.87), (-3.916, 516.0), (-3.916, 515.76), (-10.782, 516.0), (-10.782, 515.76), (-0.3, 515.87), (-0.3, 515.74), (-3.916, 515.87), (-3.916, 515.74), (-3.916, 515.63), (-10.782, 515.52), (-3.916, 515.76), (-10.782, 515.52), (-0.3, 515.74), (-0.3, 515.63), (-3.916, 515.74), (-3.916, 515.63), (-3.916, 515.63), (-10.782, 515.52), (-3.916, 515.76), (-10.782, 515.52)]</t>
+          <t>[(-0.3, 516.0), (-0.3, 515.87), (-3.916, 516.0), (-3.916, 515.87), (-3.916, 516.0), (-3.916, 515.76), (-10.782, 516.0), (-10.782, 515.76), (-0.3, 515.87), (-0.3, 515.74), (-3.916, 515.87), (-3.916, 515.74), (-3.916, 515.63), (-3.916, 515.52), (-10.782, 515.76), (-10.782, 515.52), (-0.3, 515.74), (-0.3, 515.63), (-3.916, 515.74), (-3.916, 515.63), (-3.916, 515.63), (-3.916, 515.63), (-10.782, 515.76), (-10.782, 515.52)]</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>[(-0.3, 517.0), (-0.3, 516.82), (-4.131, 517.0), (-4.131, 516.82), (-4.131, 517.0), (-4.131, 516.84), (-10.953, 517.0), (-10.953, 516.84), (-0.3, 516.82), (-0.3, 516.64), (-4.131, 516.82), (-4.131, 516.68), (-4.131, 516.68), (-10.953, 516.54), (-4.131, 516.84), (-10.953, 516.54)]</t>
+          <t>[(-0.3, 517.0), (-0.3, 516.82), (-4.131, 517.0), (-4.131, 516.82), (-4.131, 517.0), (-4.131, 516.84), (-10.953, 517.0), (-10.953, 516.84), (-0.3, 516.82), (-0.3, 516.64), (-4.131, 516.82), (-4.131, 516.68), (-4.131, 516.84), (-4.131, 516.68), (-10.953, 516.84), (-10.953, 516.54)]</t>
         </is>
       </c>
     </row>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>[(-0.3, 518.0), (-0.3, 517.8), (-4.733, 518.0), (-4.733, 517.8), (-4.733, 518.0), (-4.733, 517.71), (-11.574, 518.0), (-11.574, 517.71), (-0.3, 517.8), (-0.3, 517.65), (-4.733, 517.8), (-4.733, 517.6), (-4.733, 517.6), (-11.574, 517.42), (-4.733, 517.71), (-11.574, 517.42)]</t>
+          <t>[(-0.3, 518.0), (-0.3, 517.8), (-4.733, 518.0), (-4.733, 517.8), (-4.733, 518.0), (-4.733, 517.71), (-11.574, 518.0), (-11.574, 517.71), (-0.3, 517.8), (-0.3, 517.65), (-4.733, 517.8), (-4.733, 517.6), (-4.733, 517.71), (-4.733, 517.6), (-11.574, 517.71), (-11.574, 517.42)]</t>
         </is>
       </c>
     </row>
@@ -5617,7 +5617,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>[(-0.3, 519.0), (-0.3, 518.79), (-5.234, 519.0), (-5.234, 518.79), (-5.234, 519.0), (-5.234, 518.79), (-12.18, 519.0), (-12.18, 518.7), (-0.3, 518.79), (-0.3, 518.68), (-5.234, 518.79), (-5.234, 518.58), (-5.234, 518.58), (-12.18, 518.4), (-5.234, 518.79), (-12.18, 518.4)]</t>
+          <t>[(-0.3, 519.0), (-0.3, 518.79), (-5.234, 519.0), (-5.234, 518.79), (-5.234, 519.0), (-5.234, 518.79), (-12.18, 519.0), (-12.18, 518.7), (-0.3, 518.79), (-0.3, 518.68), (-5.234, 518.79), (-5.234, 518.58), (-5.234, 518.79), (-5.234, 518.58), (-12.18, 518.7), (-12.18, 518.4)]</t>
         </is>
       </c>
     </row>
@@ -5627,7 +5627,7 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>[(-0.3, 520.0), (-0.3, 519.78), (-5.555, 520.0), (-5.555, 519.78), (-5.555, 520.0), (-5.555, 519.7), (-12.458, 520.0), (-12.458, 519.7), (-0.3, 519.78), (-0.3, 519.66), (-5.555, 519.78), (-5.555, 519.57), (-5.555, 519.57), (-12.458, 519.41), (-5.555, 519.7), (-12.458, 519.41)]</t>
+          <t>[(-0.3, 520.0), (-0.3, 519.78), (-5.555, 520.0), (-5.555, 519.78), (-5.555, 520.0), (-5.555, 519.7), (-12.458, 520.0), (-12.458, 519.7), (-0.3, 519.78), (-0.3, 519.66), (-5.555, 519.78), (-5.555, 519.57), (-5.555, 519.7), (-5.555, 519.57), (-12.458, 519.7), (-12.458, 519.41)]</t>
         </is>
       </c>
     </row>
@@ -5637,7 +5637,7 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>[(-0.3, 521.0), (-0.3, 520.89), (-5.537, 521.0), (-5.537, 520.89), (-5.537, 521.0), (-5.537, 520.73), (-12.466, 521.0), (-12.466, 520.73), (-0.3, 520.89), (-0.3, 520.73), (-5.537, 520.89), (-5.537, 520.62), (-5.537, 520.62), (-12.466, 520.46), (-5.537, 520.73), (-12.466, 520.46)]</t>
+          <t>[(-0.3, 521.0), (-0.3, 520.89), (-5.537, 521.0), (-5.537, 520.89), (-5.537, 521.0), (-5.537, 520.73), (-12.466, 521.0), (-12.466, 520.73), (-0.3, 520.89), (-0.3, 520.73), (-5.537, 520.89), (-5.537, 520.62), (-5.537, 520.73), (-5.537, 520.62), (-12.466, 520.73), (-12.466, 520.46)]</t>
         </is>
       </c>
     </row>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>[(-0.3, 522.0), (-0.3, 521.89), (-5.217, 522.0), (-5.217, 521.89), (-5.217, 522.0), (-5.217, 521.84), (-12.168, 522.0), (-12.168, 521.74), (-0.3, 521.89), (-0.3, 521.74), (-5.217, 521.89), (-5.217, 521.67), (-5.217, 521.68), (-12.168, 521.48), (-5.217, 521.84), (-12.168, 521.48)]</t>
+          <t>[(-0.3, 522.0), (-0.3, 521.89), (-5.217, 522.0), (-5.217, 521.89), (-5.217, 522.0), (-5.217, 521.84), (-12.168, 522.0), (-12.168, 521.74), (-0.3, 521.89), (-0.3, 521.74), (-5.217, 521.89), (-5.217, 521.67), (-5.217, 521.84), (-5.217, 521.68), (-12.168, 521.74), (-12.168, 521.48)]</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5667,7 +5667,7 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5697,7 +5697,7 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5707,7 +5707,7 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5717,7 +5717,7 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5747,7 +5747,7 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5787,7 +5787,7 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5837,7 +5837,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5847,7 +5847,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5857,7 +5857,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5867,7 +5867,7 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5887,7 +5887,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5897,7 +5897,7 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5907,7 +5907,7 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5917,7 +5917,7 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5927,7 +5927,7 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5947,7 +5947,7 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5957,7 +5957,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5977,7 +5977,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5987,7 +5987,7 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -5997,7 +5997,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6007,7 +6007,7 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6057,7 +6057,7 @@
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6137,7 +6137,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6157,7 +6157,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6167,7 +6167,7 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6187,7 +6187,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6197,7 +6197,7 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6207,7 +6207,7 @@
       </c>
       <c r="B579" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6217,7 +6217,7 @@
       </c>
       <c r="B580" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="B581" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6237,7 +6237,7 @@
       </c>
       <c r="B582" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6247,7 +6247,7 @@
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6337,7 +6337,7 @@
       </c>
       <c r="B592" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6347,7 +6347,7 @@
       </c>
       <c r="B593" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6407,7 +6407,7 @@
       </c>
       <c r="B599" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="B620" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6637,7 +6637,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6767,7 +6767,7 @@
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6777,7 +6777,7 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6797,7 +6797,7 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="B639" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6817,7 +6817,7 @@
       </c>
       <c r="B640" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>
@@ -6847,7 +6847,7 @@
       </c>
       <c r="B643" t="inlineStr">
         <is>
-          <t>[0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+          <t>[0]</t>
         </is>
       </c>
     </row>

</xml_diff>